<commit_message>
numerical issue observed, not fixed yet.
</commit_message>
<xml_diff>
--- a/matrix.xlsx
+++ b/matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="29380" yWindow="0" windowWidth="13920" windowHeight="13400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8840" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="76">
   <si>
     <t>C</t>
   </si>
@@ -217,15 +217,6 @@
     <t>ct</t>
   </si>
   <si>
-    <t>Ut</t>
-  </si>
-  <si>
-    <t>Up</t>
-  </si>
-  <si>
-    <t>Ud</t>
-  </si>
-  <si>
     <t>=0</t>
   </si>
   <si>
@@ -244,10 +235,19 @@
     <t>&lt;=C0</t>
   </si>
   <si>
-    <t>vB</t>
-  </si>
-  <si>
-    <t>vC</t>
+    <t>z</t>
+  </si>
+  <si>
+    <t>&lt;=0.5</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>-A</t>
+  </si>
+  <si>
+    <t>&lt;=d</t>
   </si>
 </sst>
 </file>
@@ -976,11 +976,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ25"/>
+  <dimension ref="A1:AO25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AM7" sqref="AM7"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AL20" sqref="AL20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1005,14 +1005,13 @@
     <col min="35" max="35" width="2.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="3.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="38" width="3.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="40" width="3.1796875" style="1" customWidth="1"/>
-    <col min="41" max="41" width="4.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="3.81640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.81640625" style="28"/>
-    <col min="44" max="16384" width="8.81640625" style="1"/>
+    <col min="39" max="39" width="4.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="3.81640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.81640625" style="28"/>
+    <col min="42" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -1110,22 +1109,16 @@
         <v>64</v>
       </c>
       <c r="AJ1" s="32" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="AK1" s="30" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="AL1" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1177,20 +1170,18 @@
       <c r="AJ2" s="34"/>
       <c r="AK2" s="33"/>
       <c r="AL2" s="34"/>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="4"/>
-      <c r="AO2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP2" s="28">
+      <c r="AM2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN2" s="28">
         <v>72</v>
       </c>
-      <c r="AQ2" s="28">
-        <f>AP2</f>
+      <c r="AO2" s="28">
+        <f>AN2</f>
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1242,22 +1233,18 @@
       <c r="AJ3" s="34"/>
       <c r="AK3" s="33"/>
       <c r="AL3" s="34"/>
-      <c r="AM3" s="4"/>
-      <c r="AN3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AO3" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP3" s="28">
+      <c r="AM3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN3" s="28">
         <v>72</v>
       </c>
-      <c r="AQ3" s="28">
-        <f>AQ2+AP3</f>
+      <c r="AO3" s="28">
+        <f>AO2+AN3</f>
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1307,20 +1294,18 @@
       <c r="AL4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP4" s="28">
+      <c r="AM4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN4" s="28">
         <v>72</v>
       </c>
-      <c r="AQ4" s="28">
-        <f t="shared" ref="AQ4:AQ12" si="0">AQ3+AP4</f>
+      <c r="AO4" s="28">
+        <f t="shared" ref="AO4:AO12" si="0">AO3+AN4</f>
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="27"/>
@@ -1371,21 +1356,17 @@
       </c>
       <c r="AL5" s="34"/>
       <c r="AM5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AN5" s="4"/>
-      <c r="AO5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP5" s="28">
         <v>72</v>
       </c>
-      <c r="AQ5" s="28">
+      <c r="AN5" s="28">
+        <v>72</v>
+      </c>
+      <c r="AO5" s="28">
         <f t="shared" si="0"/>
         <v>288</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="27"/>
@@ -1436,21 +1417,17 @@
       </c>
       <c r="AL6" s="34"/>
       <c r="AM6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AN6" s="4"/>
-      <c r="AO6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP6" s="28">
         <v>72</v>
       </c>
-      <c r="AQ6" s="28">
+      <c r="AN6" s="28">
+        <v>72</v>
+      </c>
+      <c r="AO6" s="28">
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="27"/>
@@ -1498,20 +1475,18 @@
       <c r="AJ7" s="34"/>
       <c r="AK7" s="33"/>
       <c r="AL7" s="34"/>
-      <c r="AM7" s="4"/>
-      <c r="AN7" s="4"/>
-      <c r="AO7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP7" s="28">
+      <c r="AM7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AQ7" s="28">
+      <c r="AN7" s="28">
+        <v>72</v>
+      </c>
+      <c r="AO7" s="28">
         <f t="shared" si="0"/>
         <v>432</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -1559,20 +1534,18 @@
       <c r="AJ8" s="34"/>
       <c r="AK8" s="33"/>
       <c r="AL8" s="34"/>
-      <c r="AM8" s="4"/>
-      <c r="AN8" s="4"/>
-      <c r="AO8" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP8" s="28">
+      <c r="AM8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AQ8" s="28">
+      <c r="AN8" s="28">
+        <v>72</v>
+      </c>
+      <c r="AO8" s="28">
         <f t="shared" si="0"/>
         <v>504</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -1620,20 +1593,18 @@
         <v>6</v>
       </c>
       <c r="AL9" s="34"/>
-      <c r="AM9" s="4"/>
-      <c r="AN9" s="4"/>
-      <c r="AO9" s="4" t="s">
+      <c r="AM9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN9" s="28">
         <v>72</v>
       </c>
-      <c r="AP9" s="28">
-        <v>72</v>
-      </c>
-      <c r="AQ9" s="28">
+      <c r="AO9" s="28">
         <f t="shared" si="0"/>
         <v>576</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="27" t="s">
@@ -1683,20 +1654,18 @@
       <c r="AL10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AM10" s="4"/>
-      <c r="AN10" s="4"/>
-      <c r="AO10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP10" s="28">
+      <c r="AM10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN10" s="28">
         <v>72</v>
       </c>
-      <c r="AQ10" s="28">
+      <c r="AO10" s="28">
         <f t="shared" si="0"/>
         <v>648</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="27" t="s">
@@ -1744,20 +1713,18 @@
       </c>
       <c r="AK11" s="33"/>
       <c r="AL11" s="34"/>
-      <c r="AM11" s="4"/>
-      <c r="AN11" s="4"/>
-      <c r="AO11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP11" s="28">
+      <c r="AM11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN11" s="28">
         <v>72</v>
       </c>
-      <c r="AQ11" s="28">
+      <c r="AO11" s="28">
         <f t="shared" si="0"/>
         <v>720</v>
       </c>
     </row>
-    <row r="12" spans="1:43" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="25"/>
       <c r="D12" s="22"/>
       <c r="E12" s="25"/>
@@ -1787,20 +1754,18 @@
       <c r="AJ12" s="37"/>
       <c r="AK12" s="35"/>
       <c r="AL12" s="37"/>
-      <c r="AM12" s="29"/>
-      <c r="AN12" s="29"/>
-      <c r="AO12" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AP12" s="28">
+      <c r="AM12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN12" s="28">
         <v>12</v>
       </c>
-      <c r="AQ12" s="28">
+      <c r="AO12" s="28">
         <f t="shared" si="0"/>
         <v>732</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1852,15 +1817,13 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
-      <c r="AM13" s="2"/>
-      <c r="AN13" s="2"/>
-      <c r="AO13" s="29"/>
-      <c r="AP13" s="28">
-        <f>SUM(AP2:AP12)</f>
+      <c r="AM13" s="29"/>
+      <c r="AN13" s="28">
+        <f>SUM(AN2:AN12)</f>
         <v>732</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="27" t="s">
@@ -1913,10 +1876,8 @@
       <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
       <c r="AM14" s="2"/>
-      <c r="AN14" s="2"/>
-      <c r="AO14" s="2"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="27" t="s">
@@ -1957,22 +1918,31 @@
       <c r="AA15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AB15" s="2"/>
+      <c r="AB15" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
-      <c r="AE15" s="2"/>
+      <c r="AE15" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
-      <c r="AH15" s="2"/>
+      <c r="AH15" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
-      <c r="AM15" s="2"/>
-      <c r="AN15" s="2"/>
-      <c r="AO15" s="2"/>
+      <c r="AM15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN15" s="28">
+        <v>72</v>
+      </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
@@ -2014,20 +1984,29 @@
         <v>38</v>
       </c>
       <c r="AB16" s="2"/>
-      <c r="AC16" s="2"/>
+      <c r="AC16" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="AE16" s="2"/>
-      <c r="AF16" s="2"/>
+      <c r="AF16" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
-      <c r="AI16" s="2"/>
+      <c r="AI16" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="2"/>
-      <c r="AM16" s="2"/>
-      <c r="AN16" s="2"/>
-      <c r="AO16" s="2"/>
+      <c r="AM16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN16" s="28">
+        <v>144</v>
+      </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -2065,22 +2044,29 @@
       <c r="Y17" s="28">
         <v>72</v>
       </c>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="2"/>
-      <c r="AD17" s="2"/>
-      <c r="AE17" s="2"/>
-      <c r="AF17" s="2"/>
-      <c r="AG17" s="2"/>
-      <c r="AH17" s="2"/>
-      <c r="AI17" s="2"/>
-      <c r="AJ17" s="2"/>
-      <c r="AK17" s="2"/>
-      <c r="AL17" s="2"/>
-      <c r="AM17" s="2"/>
-      <c r="AN17" s="2"/>
-      <c r="AO17" s="2"/>
+      <c r="AB17" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD17" s="34"/>
+      <c r="AE17" s="33"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="34"/>
+      <c r="AH17" s="33"/>
+      <c r="AI17" s="4"/>
+      <c r="AJ17" s="34"/>
+      <c r="AK17" s="33"/>
+      <c r="AL17" s="34"/>
+      <c r="AM17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN17" s="28">
+        <v>216</v>
+      </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
@@ -2116,22 +2102,29 @@
       <c r="Y18" s="28">
         <v>72</v>
       </c>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="2"/>
-      <c r="AD18" s="2"/>
-      <c r="AE18" s="2"/>
-      <c r="AF18" s="2"/>
-      <c r="AG18" s="2"/>
-      <c r="AH18" s="2"/>
-      <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2"/>
-      <c r="AL18" s="2"/>
-      <c r="AM18" s="2"/>
-      <c r="AN18" s="2"/>
-      <c r="AO18" s="2"/>
+      <c r="AB18" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD18" s="34"/>
+      <c r="AE18" s="33"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="34"/>
+      <c r="AH18" s="33"/>
+      <c r="AI18" s="4"/>
+      <c r="AJ18" s="34"/>
+      <c r="AK18" s="33"/>
+      <c r="AL18" s="34"/>
+      <c r="AM18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN18" s="28">
+        <v>288</v>
+      </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -2167,8 +2160,17 @@
       <c r="Y19" s="28">
         <v>72</v>
       </c>
+      <c r="AH19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN19" s="28">
+        <v>360</v>
+      </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="27"/>
@@ -2202,8 +2204,20 @@
       <c r="Y20" s="28">
         <v>72</v>
       </c>
+      <c r="AB20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN20" s="28">
+        <v>372</v>
+      </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="27"/>
@@ -2240,7 +2254,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="27"/>
@@ -2277,7 +2291,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="27"/>
@@ -2314,7 +2328,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
         <v>60</v>
@@ -2349,7 +2363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="Y25" s="28">
         <f>SUM(Y13:Y24)</f>
         <v>804</v>

</xml_diff>